<commit_message>
Se corrige errores en DB y cosas menores
</commit_message>
<xml_diff>
--- a/backend_test/etiquetado.xlsx
+++ b/backend_test/etiquetado.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9def1edecff34b88/UNIR_Edgar/proyecto_placas/backend_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="398" documentId="11_0705D3ACD3C0D2372F582211595ED87656CD1EEE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CA72297-790F-4F2E-B371-18964A844F84}"/>
+  <xr:revisionPtr revIDLastSave="498" documentId="11_0705D3ACD3C0D2372F582211595ED87656CD1EEE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E7AAB89-AE60-41E2-A0B0-82E25707710E}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="257">
   <si>
     <t>auto_01.png</t>
   </si>
@@ -710,6 +710,87 @@
   </si>
   <si>
     <t>FUIE 419</t>
+  </si>
+  <si>
+    <t>BL1155</t>
+  </si>
+  <si>
+    <t>PY</t>
+  </si>
+  <si>
+    <t>MH 20 EE 7601</t>
+  </si>
+  <si>
+    <t>MH 20EE 7601</t>
+  </si>
+  <si>
+    <t>MH 03 BS 7778</t>
+  </si>
+  <si>
+    <t>MH03BS 7778</t>
+  </si>
+  <si>
+    <t>KL 02</t>
+  </si>
+  <si>
+    <t>TN 74 AL 5074</t>
+  </si>
+  <si>
+    <t>TNZLAL 5074</t>
+  </si>
+  <si>
+    <t>8117 MP-7</t>
+  </si>
+  <si>
+    <t>8117MP-]</t>
+  </si>
+  <si>
+    <t>KA 29 Z 999</t>
+  </si>
+  <si>
+    <t>AND</t>
+  </si>
+  <si>
+    <t>KL 53E 964</t>
+  </si>
+  <si>
+    <t>KL: 53E 964</t>
+  </si>
+  <si>
+    <t>TN 45 BA 1065</t>
+  </si>
+  <si>
+    <t>IH45 BA 1065</t>
+  </si>
+  <si>
+    <t>ME 9869</t>
+  </si>
+  <si>
+    <t>9869_</t>
+  </si>
+  <si>
+    <t>KL07CB8599</t>
+  </si>
+  <si>
+    <t>[ALDZIBESGG</t>
+  </si>
+  <si>
+    <t>HR.26 BR.9044</t>
+  </si>
+  <si>
+    <t>HR.26.BR.9044</t>
+  </si>
+  <si>
+    <t>PERLA</t>
+  </si>
+  <si>
+    <t>MH 14 EH 7958</t>
+  </si>
+  <si>
+    <t>FHH 14EH7958</t>
+  </si>
+  <si>
+    <t>COBRE</t>
   </si>
 </sst>
 </file>
@@ -776,14 +857,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -799,6 +881,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1088,8 +1174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2344,88 +2430,376 @@
       <c r="A47" t="s">
         <v>45</v>
       </c>
+      <c r="B47" t="s">
+        <v>133</v>
+      </c>
+      <c r="C47" t="s">
+        <v>230</v>
+      </c>
+      <c r="D47" t="s">
+        <v>168</v>
+      </c>
+      <c r="E47" t="s">
+        <v>145</v>
+      </c>
+      <c r="F47">
+        <v>3.3</v>
+      </c>
+      <c r="G47" t="s">
+        <v>133</v>
+      </c>
+      <c r="H47" t="s">
+        <v>231</v>
+      </c>
+      <c r="I47" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>133</v>
+      </c>
+      <c r="C48" t="s">
+        <v>232</v>
+      </c>
+      <c r="D48" t="s">
+        <v>147</v>
+      </c>
+      <c r="F48">
+        <v>3</v>
+      </c>
+      <c r="G48" t="s">
+        <v>133</v>
+      </c>
+      <c r="H48" t="s">
+        <v>233</v>
+      </c>
+      <c r="I48" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>133</v>
+      </c>
+      <c r="C49" t="s">
+        <v>234</v>
+      </c>
+      <c r="D49" t="s">
+        <v>147</v>
+      </c>
+      <c r="F49">
+        <v>3.2</v>
+      </c>
+      <c r="G49" t="s">
+        <v>133</v>
+      </c>
+      <c r="H49" t="s">
+        <v>235</v>
+      </c>
+      <c r="I49" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>174</v>
+      </c>
+      <c r="C50" t="s">
+        <v>236</v>
+      </c>
+      <c r="D50" t="s">
+        <v>147</v>
+      </c>
+      <c r="E50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F50">
+        <v>3.2</v>
+      </c>
+      <c r="G50" t="s">
+        <v>133</v>
+      </c>
+      <c r="H50" t="s">
+        <v>236</v>
+      </c>
+      <c r="I50" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>133</v>
+      </c>
+      <c r="C51" t="s">
+        <v>237</v>
+      </c>
+      <c r="D51" t="s">
+        <v>168</v>
+      </c>
+      <c r="F51">
+        <v>3.5</v>
+      </c>
+      <c r="G51" t="s">
+        <v>133</v>
+      </c>
+      <c r="H51" t="s">
+        <v>238</v>
+      </c>
+      <c r="I51" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>133</v>
+      </c>
+      <c r="C52" t="s">
+        <v>239</v>
+      </c>
+      <c r="D52" t="s">
+        <v>147</v>
+      </c>
+      <c r="E52" t="s">
+        <v>144</v>
+      </c>
+      <c r="F52">
+        <v>3</v>
+      </c>
+      <c r="G52" t="s">
+        <v>133</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="I52" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>133</v>
+      </c>
+      <c r="C53" t="s">
+        <v>241</v>
+      </c>
+      <c r="D53" t="s">
+        <v>132</v>
+      </c>
+      <c r="E53" t="s">
+        <v>146</v>
+      </c>
+      <c r="F53">
+        <v>3.8</v>
+      </c>
+      <c r="G53" t="s">
+        <v>133</v>
+      </c>
+      <c r="H53" t="s">
+        <v>242</v>
+      </c>
+      <c r="I53" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>174</v>
+      </c>
+      <c r="C54" t="s">
+        <v>243</v>
+      </c>
+      <c r="D54" t="s">
+        <v>168</v>
+      </c>
+      <c r="F54">
+        <v>3</v>
+      </c>
+      <c r="G54" t="s">
+        <v>133</v>
+      </c>
+      <c r="H54" t="s">
+        <v>244</v>
+      </c>
+      <c r="I54" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>174</v>
+      </c>
+      <c r="C55" t="s">
+        <v>245</v>
+      </c>
+      <c r="D55" t="s">
+        <v>132</v>
+      </c>
+      <c r="F55">
+        <v>3.1</v>
+      </c>
+      <c r="G55" t="s">
+        <v>133</v>
+      </c>
+      <c r="H55" t="s">
+        <v>246</v>
+      </c>
+      <c r="I55" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>133</v>
+      </c>
+      <c r="C56" t="s">
+        <v>247</v>
+      </c>
+      <c r="D56" t="s">
+        <v>132</v>
+      </c>
+      <c r="E56" t="s">
+        <v>144</v>
+      </c>
+      <c r="F56">
+        <v>2.8</v>
+      </c>
+      <c r="G56" t="s">
+        <v>133</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="I56" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>133</v>
+      </c>
+      <c r="C57" t="s">
+        <v>249</v>
+      </c>
+      <c r="D57" t="s">
+        <v>132</v>
+      </c>
+      <c r="F57">
+        <v>3</v>
+      </c>
+      <c r="G57" t="s">
+        <v>133</v>
+      </c>
+      <c r="H57" t="s">
+        <v>250</v>
+      </c>
+      <c r="I57" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>133</v>
+      </c>
+      <c r="C58" t="s">
+        <v>252</v>
+      </c>
+      <c r="D58" t="s">
+        <v>163</v>
+      </c>
+      <c r="F58">
+        <v>2.9</v>
+      </c>
+      <c r="G58" t="s">
+        <v>174</v>
+      </c>
+      <c r="H58" t="s">
+        <v>251</v>
+      </c>
+      <c r="I58" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>133</v>
+      </c>
+      <c r="C59" t="s">
+        <v>254</v>
+      </c>
+      <c r="D59" t="s">
+        <v>163</v>
+      </c>
+      <c r="F59">
+        <v>2.7</v>
+      </c>
+      <c r="G59" t="s">
+        <v>133</v>
+      </c>
+      <c r="H59" t="s">
+        <v>255</v>
+      </c>
+      <c r="I59" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>62</v>
       </c>

</xml_diff>